<commit_message>
Mise à jour cases.xlsx
</commit_message>
<xml_diff>
--- a/ideas/cases.xlsx
+++ b/ideas/cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\RadiUm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\wamp\www\pji\M1S2_PJI\ideas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Empty</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>tree_type</t>
+  </si>
+  <si>
+    <t>water_received</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,14 +118,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,85 +423,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="14" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>